<commit_message>
atualizando códigos (loop teste) e resultados.
</commit_message>
<xml_diff>
--- a/resultados(logs_saidas)/resultadosAlexNet/models_metrics.xlsx
+++ b/resultados(logs_saidas)/resultadosAlexNet/models_metrics.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0133337242297736</v>
+        <v>0.01222129826550129</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9957916666666666</v>
+        <v>0.9966874999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0516950312067346</v>
+        <v>0.03400449777442152</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9875833333333334</v>
+        <v>0.9905833333333334</v>
       </c>
       <c r="F2" t="n">
-        <v>496.501354</v>
+        <v>488.926047</v>
       </c>
       <c r="G2" t="n">
-        <v>87.256</v>
+        <v>86.752</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.013401185424634</v>
+        <v>0.01330745655684708</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9959895833333333</v>
+        <v>0.9962916666666666</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04504525618358698</v>
+        <v>0.03533847363175308</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9886250000000001</v>
+        <v>0.9903333333333333</v>
       </c>
       <c r="F3" t="n">
-        <v>482.541859</v>
+        <v>486.714349</v>
       </c>
       <c r="G3" t="n">
-        <v>87.28100000000001</v>
+        <v>87.578</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01365568300724044</v>
+        <v>0.01349757201275821</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9958541666666667</v>
+        <v>0.9960624999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04523311213725358</v>
+        <v>0.03955140594994933</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9881666666666667</v>
+        <v>0.9894722222222222</v>
       </c>
       <c r="F4" t="n">
-        <v>480.79168</v>
+        <v>481.579698</v>
       </c>
       <c r="G4" t="n">
-        <v>87.667</v>
+        <v>87.358</v>
       </c>
     </row>
     <row r="5">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01328831710375107</v>
+        <v>0.01342514414958926</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9959791666666666</v>
+        <v>0.9959583333333333</v>
       </c>
       <c r="D5" t="n">
-        <v>0.04574180978583525</v>
+        <v>0.04085397449813036</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9882916666666667</v>
+        <v>0.9892083333333334</v>
       </c>
       <c r="F5" t="n">
-        <v>480.560282</v>
+        <v>480.298261</v>
       </c>
       <c r="G5" t="n">
-        <v>87.529</v>
+        <v>87.39700000000001</v>
       </c>
     </row>
     <row r="6">
@@ -577,22 +577,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01300265827286373</v>
+        <v>0.01298716859576598</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9960458333333333</v>
+        <v>0.9961208333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04431977491540214</v>
+        <v>0.04054353564209103</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9889666666666667</v>
+        <v>0.9893666666666666</v>
       </c>
       <c r="F6" t="n">
-        <v>479.49993</v>
+        <v>480.393492</v>
       </c>
       <c r="G6" t="n">
-        <v>87.78700000000001</v>
+        <v>87.486</v>
       </c>
     </row>
     <row r="7">
@@ -602,22 +602,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01321161453224037</v>
+        <v>0.01287015847688175</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9960069444444445</v>
+        <v>0.9961701388888889</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04389502741978821</v>
+        <v>0.04085544673555932</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9890694444444444</v>
+        <v>0.9893611111111111</v>
       </c>
       <c r="F7" t="n">
-        <v>477.997565</v>
+        <v>482.989044</v>
       </c>
       <c r="G7" t="n">
-        <v>88.021</v>
+        <v>86.685</v>
       </c>
     </row>
     <row r="8">
@@ -627,22 +627,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01303147935201958</v>
+        <v>0.01280095153107175</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9960654761904763</v>
+        <v>0.9961994047619047</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04265030976048182</v>
+        <v>0.04014146601044533</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9894285714285714</v>
+        <v>0.9896785714285715</v>
       </c>
       <c r="F8" t="n">
-        <v>479.871528</v>
+        <v>487.935808</v>
       </c>
       <c r="G8" t="n">
-        <v>87.60899999999999</v>
+        <v>87.48</v>
       </c>
     </row>
     <row r="9">
@@ -652,22 +652,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01309860517669904</v>
+        <v>0.01280084208583996</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9960390625</v>
+        <v>0.9961979166666666</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04444268784804419</v>
+        <v>0.03979258810414816</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9890833333333333</v>
+        <v>0.9898125</v>
       </c>
       <c r="F9" t="n">
-        <v>480.138173</v>
+        <v>482.874725</v>
       </c>
       <c r="G9" t="n">
-        <v>87.214</v>
+        <v>86.952</v>
       </c>
     </row>
     <row r="10">
@@ -677,22 +677,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01289298439493925</v>
+        <v>0.01272892271442571</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9961064814814815</v>
+        <v>0.9962291666666666</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0434578655803011</v>
+        <v>0.03870231707399497</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9894722222222223</v>
+        <v>0.9899907407407407</v>
       </c>
       <c r="F10" t="n">
-        <v>480.097193</v>
+        <v>490.74664</v>
       </c>
       <c r="G10" t="n">
-        <v>88.14400000000001</v>
+        <v>85.93899999999999</v>
       </c>
     </row>
     <row r="11">
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01298296638639392</v>
+        <v>0.012552012262605</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9960770833333333</v>
+        <v>0.9962583333333332</v>
       </c>
       <c r="D11" t="n">
-        <v>0.04330564696884187</v>
+        <v>0.03807468705323368</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9895416666666668</v>
+        <v>0.9901416666666666</v>
       </c>
       <c r="F11" t="n">
-        <v>478.83235</v>
+        <v>491.263767</v>
       </c>
       <c r="G11" t="n">
-        <v>87.485</v>
+        <v>86.85899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>